<commit_message>
Suck on LH plot
</commit_message>
<xml_diff>
--- a/Spring/LifeHistoryTable.xlsx
+++ b/Spring/LifeHistoryTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\johnson_capstone\Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED52660-DEA1-49AE-9D1C-B139DBFBE3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C85E65-6375-4049-8144-BD0F570721AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3505ECB3-DA55-4A5D-9DB9-B935B09950CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Eggs</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Spawning</t>
   </si>
   <si>
-    <t>Adult Survival</t>
-  </si>
-  <si>
     <t>MinTemp</t>
   </si>
   <si>
@@ -63,6 +60,24 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>01, 02, 03, 11, 12</t>
+  </si>
+  <si>
+    <t>02, 03, 04</t>
+  </si>
+  <si>
+    <t>06, 07, 09, 09, 10</t>
+  </si>
+  <si>
+    <t>09, 10, 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LH_Stage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month </t>
   </si>
 </sst>
 </file>
@@ -434,114 +449,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633AAFA6-C280-4772-9ECC-93C47CFBEE98}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B10" sqref="B10:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
         <v>-3.1970000000000001</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>11.528</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4.0784921185154497</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2.4001288794104401</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
         <v>-1.456</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>17.95</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4.6695105337078697</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3.02052130260072</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
         <v>5.6550000000000002</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>20.138000000000002</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>13.7522661626928</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2.7718664686113899</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>2.8370000000000002</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>18.901</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>10.149747052426701</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3.1867817403018002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>8.3819999999999997</v>
-      </c>
-      <c r="C7">
-        <v>20.138000000000002</v>
-      </c>
-      <c r="D7">
-        <v>14.759090119541399</v>
-      </c>
-      <c r="E7">
-        <v>1.95330472048027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Progress, but not with model plots
</commit_message>
<xml_diff>
--- a/Spring/LifeHistoryTable.xlsx
+++ b/Spring/LifeHistoryTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\johnson_capstone\Spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C85E65-6375-4049-8144-BD0F570721AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3629D4E7-DF34-48C1-BA57-C6C9F70070A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3505ECB3-DA55-4A5D-9DB9-B935B09950CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{3505ECB3-DA55-4A5D-9DB9-B935B09950CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Eggs</t>
   </si>
@@ -47,9 +47,6 @@
     <t>YOY</t>
   </si>
   <si>
-    <t>Spawning</t>
-  </si>
-  <si>
     <t>MinTemp</t>
   </si>
   <si>
@@ -62,22 +59,31 @@
     <t>SD</t>
   </si>
   <si>
-    <t>01, 02, 03, 11, 12</t>
-  </si>
-  <si>
-    <t>02, 03, 04</t>
-  </si>
-  <si>
-    <t>06, 07, 09, 09, 10</t>
-  </si>
-  <si>
-    <t>09, 10, 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LH_Stage </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Month </t>
+    <t>November 2020 to March 2021</t>
+  </si>
+  <si>
+    <t>February to April 2021</t>
+  </si>
+  <si>
+    <t>June to October 2020</t>
+  </si>
+  <si>
+    <t>September to November 2020</t>
+  </si>
+  <si>
+    <t>LH_Stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spawning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adult Survival </t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>June to August 2020 to 2021</t>
   </si>
 </sst>
 </file>
@@ -449,44 +455,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633AAFA6-C280-4772-9ECC-93C47CFBEE98}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B14"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.90625" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="9" max="9" width="25.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>-3.1970000000000001</v>
@@ -501,12 +509,12 @@
         <v>2.4001288794104401</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>-1.456</v>
@@ -521,12 +529,12 @@
         <v>3.02052130260072</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>5.6550000000000002</v>
@@ -541,12 +549,12 @@
         <v>2.7718664686113899</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>2.8370000000000002</v>
@@ -559,6 +567,26 @@
       </c>
       <c r="F5">
         <v>3.1867817403018002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>8.3819999999999997</v>
+      </c>
+      <c r="D6">
+        <v>20.138000000000002</v>
+      </c>
+      <c r="E6">
+        <v>14.759090119541399</v>
+      </c>
+      <c r="F6">
+        <v>1.95330472048027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>